<commit_message>
Finish the excel to kamer pojo deserializer
</commit_message>
<xml_diff>
--- a/Hotel kamers v0.1.xlsx
+++ b/Hotel kamers v0.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jkalloe\Documents\Cursussen\Software Engineering Track\Java\reserveringssysteem-spring\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1ACED4FF-AE5B-40C1-9ACB-F8F67C01A7F5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC781FA3-A27C-4723-8C1C-4CCFB86E58C1}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{159596B7-B20F-4450-9AD4-0E1557652CEB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="16">
   <si>
     <t>Room</t>
   </si>
@@ -68,22 +68,19 @@
     <t>Disabled room</t>
   </si>
   <si>
-    <t>2 Double bed 1 single bed, 1 baby bed</t>
-  </si>
-  <si>
     <t xml:space="preserve">2 x Double </t>
   </si>
   <si>
     <t>Penthouse</t>
   </si>
   <si>
-    <t>2 x Double bed, 4 singles, 2 baby beds</t>
-  </si>
-  <si>
     <t>2 Double bed ,1 single bed, 1 baby bed</t>
   </si>
   <si>
     <t>2 Double bed, 1 single bed, 1 baby bed</t>
+  </si>
+  <si>
+    <t>2 Double bed, 4 single, 2 baby bed</t>
   </si>
 </sst>
 </file>
@@ -486,7 +483,7 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:E20"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -808,7 +805,7 @@
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B20" s="1">
         <v>4</v>
@@ -817,7 +814,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E20" s="1"/>
     </row>
@@ -837,6 +834,9 @@
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="29.5546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
@@ -1136,7 +1136,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="1">
         <v>4</v>
@@ -1145,7 +1145,7 @@
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="2"/>
@@ -1176,11 +1176,12 @@
   <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="24" customWidth="1"/>
     <col min="5" max="5" width="31.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1434,7 +1435,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B16" s="1">
         <v>4</v>
@@ -1443,7 +1444,7 @@
         <v>2</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="2"/>
@@ -1522,7 +1523,7 @@
   <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E20"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1811,7 +1812,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B19" s="1">
         <v>8</v>
@@ -1820,13 +1821,13 @@
         <v>2</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="1">
         <v>8</v>
@@ -1835,7 +1836,7 @@
         <v>2</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E20" s="1"/>
     </row>

</xml_diff>